<commit_message>
TS 7.4 7.5 Padam template - 16/03/2023
</commit_message>
<xml_diff>
--- a/TS Jatai Working/Padam Input Templates/TS 7.4 Padam Input Template.xlsx
+++ b/TS Jatai Working/Padam Input Templates/TS 7.4 Padam Input Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\texts\TS Jatai Working\Padam Input Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EB79691-F7B8-4420-8B60-AA1DF7FECD08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5479F02F-3EEA-4512-8E3C-1436EF2FA9B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7017" uniqueCount="1515">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6994" uniqueCount="1512">
   <si>
     <t>Passage</t>
   </si>
@@ -4299,9 +4299,6 @@
     <t>priqyAm</t>
   </si>
   <si>
-    <t>maqmA(4)~Mm</t>
-  </si>
-  <si>
     <t>praqjAqpaqteq</t>
   </si>
   <si>
@@ -4509,12 +4506,6 @@
     <t>aqjAqyaqthAq itya#jAyathAH</t>
   </si>
   <si>
-    <t>SE?</t>
-  </si>
-  <si>
-    <t>RE?</t>
-  </si>
-  <si>
     <t xml:space="preserve">te </t>
   </si>
   <si>
@@ -4530,15 +4521,6 @@
     <t>S[s]</t>
   </si>
   <si>
-    <t>?</t>
-  </si>
-  <si>
-    <t>NSE?</t>
-  </si>
-  <si>
-    <t>SE??</t>
-  </si>
-  <si>
     <t>Sh</t>
   </si>
   <si>
@@ -4557,9 +4539,6 @@
     <t>NSE</t>
   </si>
   <si>
-    <t>SE?RE?</t>
-  </si>
-  <si>
     <t>N[r]</t>
   </si>
   <si>
@@ -4573,13 +4552,25 @@
   </si>
   <si>
     <t>aqnvAro#hanti</t>
+  </si>
+  <si>
+    <t>P[s]</t>
+  </si>
+  <si>
+    <t>P[r]+S[r]</t>
+  </si>
+  <si>
+    <t>P[r]+N[r]</t>
+  </si>
+  <si>
+    <t>maqmA(4)~M</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="23" x14ac:knownFonts="1">
+  <fonts count="24" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -4720,8 +4711,15 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -4737,18 +4735,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="2" tint="-9.9978637043366805E-2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF00B0F0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF0070C0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -4963,20 +4949,20 @@
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="21" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -5260,15 +5246,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V2728"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1337" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="L1" sqref="L1"/>
-      <selection pane="bottomLeft" activeCell="N1335" sqref="N1335"/>
+      <selection pane="bottomLeft" activeCell="N2619" sqref="N2619"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.140625" style="2" customWidth="1"/>
+    <col min="1" max="1" width="14.28515625" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.140625" style="2" customWidth="1"/>
     <col min="3" max="3" width="11.28515625" style="5" customWidth="1"/>
     <col min="4" max="4" width="13.7109375" style="24" customWidth="1"/>
@@ -7737,7 +7723,7 @@
         <f t="shared" si="2"/>
         <v>50</v>
       </c>
-      <c r="N51" s="61" t="s">
+      <c r="N51" s="59" t="s">
         <v>164</v>
       </c>
       <c r="O51" s="7"/>
@@ -11112,7 +11098,7 @@
         <f t="shared" si="8"/>
         <v>145</v>
       </c>
-      <c r="N146" s="61" t="s">
+      <c r="N146" s="59" t="s">
         <v>1382</v>
       </c>
       <c r="O146" s="8" t="s">
@@ -11127,7 +11113,7 @@
       <c r="T146" s="8"/>
       <c r="U146" s="8"/>
       <c r="V146" s="48" t="s">
-        <v>1431</v>
+        <v>1430</v>
       </c>
     </row>
     <row r="147" spans="4:22" s="5" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -19815,7 +19801,7 @@
         <f t="shared" si="20"/>
         <v>260</v>
       </c>
-      <c r="N406" s="62" t="s">
+      <c r="N406" s="60" t="s">
         <v>205</v>
       </c>
       <c r="O406" s="7" t="s">
@@ -19851,7 +19837,7 @@
         <f t="shared" si="20"/>
         <v>261</v>
       </c>
-      <c r="N407" s="62" t="s">
+      <c r="N407" s="60" t="s">
         <v>222</v>
       </c>
       <c r="O407" s="8" t="s">
@@ -20308,7 +20294,7 @@
       <c r="T420" s="8"/>
       <c r="U420" s="8"/>
       <c r="V420" s="48" t="s">
-        <v>1431</v>
+        <v>1430</v>
       </c>
     </row>
     <row r="421" spans="4:22" s="5" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -23674,7 +23660,7 @@
         <f t="shared" si="26"/>
         <v>100</v>
       </c>
-      <c r="N520" s="61" t="s">
+      <c r="N520" s="59" t="s">
         <v>172</v>
       </c>
       <c r="O520" s="7"/>
@@ -24884,7 +24870,7 @@
         <v>85</v>
       </c>
       <c r="T555" s="8" t="s">
-        <v>1511</v>
+        <v>1504</v>
       </c>
       <c r="U555" s="8"/>
       <c r="V555" s="48"/>
@@ -30359,7 +30345,7 @@
       <c r="T719" s="8"/>
       <c r="U719" s="8"/>
       <c r="V719" s="48" t="s">
-        <v>1431</v>
+        <v>1430</v>
       </c>
     </row>
     <row r="720" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -33593,7 +33579,7 @@
         <f t="shared" si="38"/>
         <v>100</v>
       </c>
-      <c r="N819" s="61" t="s">
+      <c r="N819" s="59" t="s">
         <v>201</v>
       </c>
       <c r="O819" s="7"/>
@@ -35646,7 +35632,7 @@
         <v>163</v>
       </c>
       <c r="N882" s="48" t="s">
-        <v>1495</v>
+        <v>1492</v>
       </c>
       <c r="O882" s="7" t="s">
         <v>75</v>
@@ -35658,7 +35644,7 @@
       <c r="T882" s="8"/>
       <c r="U882" s="8"/>
       <c r="V882" s="48" t="s">
-        <v>1496</v>
+        <v>1493</v>
       </c>
     </row>
     <row r="883" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -35951,7 +35937,7 @@
       <c r="T891" s="8"/>
       <c r="U891" s="8"/>
       <c r="V891" s="48" t="s">
-        <v>1431</v>
+        <v>1430</v>
       </c>
     </row>
     <row r="892" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -37612,10 +37598,10 @@
       <c r="Q942" s="8"/>
       <c r="R942" s="8"/>
       <c r="S942" s="8" t="s">
-        <v>1497</v>
+        <v>1494</v>
       </c>
       <c r="T942" s="8" t="s">
-        <v>1498</v>
+        <v>1495</v>
       </c>
       <c r="U942" s="8"/>
       <c r="V942" s="48"/>
@@ -37718,10 +37704,10 @@
       <c r="Q945" s="8"/>
       <c r="R945" s="8"/>
       <c r="S945" s="8" t="s">
-        <v>1497</v>
+        <v>1494</v>
       </c>
       <c r="T945" s="8" t="s">
-        <v>1498</v>
+        <v>1495</v>
       </c>
       <c r="U945" s="8"/>
       <c r="V945" s="48"/>
@@ -43066,7 +43052,7 @@
         <f t="shared" si="53"/>
         <v>217</v>
       </c>
-      <c r="N1108" s="61" t="s">
+      <c r="N1108" s="59" t="s">
         <v>1382</v>
       </c>
       <c r="O1108" s="8" t="s">
@@ -43081,7 +43067,7 @@
       <c r="T1108" s="8"/>
       <c r="U1108" s="8"/>
       <c r="V1108" s="48" t="s">
-        <v>1431</v>
+        <v>1430</v>
       </c>
     </row>
     <row r="1109" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -44978,7 +44964,7 @@
         <v>59</v>
       </c>
       <c r="N1167" s="48" t="s">
-        <v>1512</v>
+        <v>1505</v>
       </c>
       <c r="O1167" s="8" t="s">
         <v>73</v>
@@ -47440,7 +47426,7 @@
         <f t="shared" si="59"/>
         <v>136</v>
       </c>
-      <c r="N1244" s="61" t="s">
+      <c r="N1244" s="59" t="s">
         <v>1382</v>
       </c>
       <c r="O1244" s="8" t="s">
@@ -47455,7 +47441,7 @@
       <c r="T1244" s="8"/>
       <c r="U1244" s="8"/>
       <c r="V1244" s="48" t="s">
-        <v>1431</v>
+        <v>1430</v>
       </c>
     </row>
     <row r="1245" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -48695,7 +48681,7 @@
         <v>39</v>
       </c>
       <c r="N1283" s="48" t="s">
-        <v>1513</v>
+        <v>1506</v>
       </c>
       <c r="O1283" s="8" t="s">
         <v>73</v>
@@ -49310,10 +49296,10 @@
       <c r="Q1302" s="8"/>
       <c r="R1302" s="8"/>
       <c r="S1302" s="8" t="s">
-        <v>1497</v>
+        <v>1494</v>
       </c>
       <c r="T1302" s="8" t="s">
-        <v>1498</v>
+        <v>1495</v>
       </c>
       <c r="U1302" s="8"/>
       <c r="V1302" s="48"/>
@@ -50199,7 +50185,7 @@
         <v>85</v>
       </c>
       <c r="N1329" s="48" t="s">
-        <v>1514</v>
+        <v>1507</v>
       </c>
       <c r="O1329" s="8" t="s">
         <v>73</v>
@@ -50709,7 +50695,7 @@
         <f t="shared" si="62"/>
         <v>100</v>
       </c>
-      <c r="N1344" s="61" t="s">
+      <c r="N1344" s="59" t="s">
         <v>337</v>
       </c>
       <c r="O1344" s="7"/>
@@ -51705,9 +51691,7 @@
       <c r="R1374" s="8"/>
       <c r="S1374" s="8"/>
       <c r="T1374" s="8"/>
-      <c r="U1374" s="8" t="s">
-        <v>1493</v>
-      </c>
+      <c r="U1374" s="8"/>
       <c r="V1374" s="48" t="s">
         <v>1245</v>
       </c>
@@ -53107,7 +53091,7 @@
         <f t="shared" si="68"/>
         <v>172</v>
       </c>
-      <c r="N1416" s="58" t="s">
+      <c r="N1416" s="48" t="s">
         <v>1382</v>
       </c>
       <c r="O1416" s="8" t="s">
@@ -53122,7 +53106,7 @@
       <c r="T1416" s="8"/>
       <c r="U1416" s="8"/>
       <c r="V1416" s="48" t="s">
-        <v>1431</v>
+        <v>1430</v>
       </c>
     </row>
     <row r="1417" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -57019,7 +57003,7 @@
         <v>100</v>
       </c>
       <c r="T1530" s="8" t="s">
-        <v>1499</v>
+        <v>1496</v>
       </c>
       <c r="U1530" s="8"/>
       <c r="V1530" s="48"/>
@@ -57261,7 +57245,7 @@
         <v>100</v>
       </c>
       <c r="T1537" s="8" t="s">
-        <v>1499</v>
+        <v>1496</v>
       </c>
       <c r="U1537" s="8"/>
       <c r="V1537" s="48"/>
@@ -57451,9 +57435,7 @@
       <c r="R1543" s="8"/>
       <c r="S1543" s="8"/>
       <c r="T1543" s="8"/>
-      <c r="U1543" s="8" t="s">
-        <v>1494</v>
-      </c>
+      <c r="U1543" s="8"/>
       <c r="V1543" s="48"/>
     </row>
     <row r="1544" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -57610,9 +57592,7 @@
       <c r="R1548" s="8"/>
       <c r="S1548" s="8"/>
       <c r="T1548" s="8"/>
-      <c r="U1548" s="8" t="s">
-        <v>1494</v>
-      </c>
+      <c r="U1548" s="8"/>
       <c r="V1548" s="48"/>
     </row>
     <row r="1549" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -57678,7 +57658,7 @@
       <c r="T1550" s="8"/>
       <c r="U1550" s="8"/>
       <c r="V1550" s="48" t="s">
-        <v>1432</v>
+        <v>1431</v>
       </c>
     </row>
     <row r="1551" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -57963,7 +57943,7 @@
         <f t="shared" si="74"/>
         <v>9</v>
       </c>
-      <c r="N1559" s="48" t="s">
+      <c r="N1559" s="52" t="s">
         <v>543</v>
       </c>
       <c r="O1559" s="8" t="s">
@@ -57974,9 +57954,7 @@
       <c r="R1559" s="8"/>
       <c r="S1559" s="8"/>
       <c r="T1559" s="8"/>
-      <c r="U1559" s="8" t="s">
-        <v>1494</v>
-      </c>
+      <c r="U1559" s="8"/>
       <c r="V1559" s="48"/>
     </row>
     <row r="1560" spans="5:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -58001,7 +57979,7 @@
         <f t="shared" si="74"/>
         <v>10</v>
       </c>
-      <c r="N1560" s="48" t="s">
+      <c r="N1560" s="52" t="s">
         <v>629</v>
       </c>
       <c r="O1560" s="7"/>
@@ -58911,10 +58889,10 @@
       <c r="N1591" s="48" t="s">
         <v>408</v>
       </c>
-      <c r="S1591" s="1" t="s">
+      <c r="S1591" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="T1591" s="1" t="s">
+      <c r="T1591" s="8" t="s">
         <v>83</v>
       </c>
       <c r="V1591" s="48"/>
@@ -59019,9 +58997,6 @@
       <c r="O1595" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="U1595" s="1" t="s">
-        <v>1494</v>
-      </c>
       <c r="V1595" s="48" t="s">
         <v>1111</v>
       </c>
@@ -59146,14 +59121,14 @@
         <f t="shared" si="74"/>
         <v>50</v>
       </c>
-      <c r="N1600" s="48" t="s">
+      <c r="N1600" s="52" t="s">
         <v>138</v>
       </c>
       <c r="P1600" s="8" t="s">
         <v>74</v>
       </c>
       <c r="V1600" s="48" t="s">
-        <v>1433</v>
+        <v>1432</v>
       </c>
     </row>
     <row r="1601" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -59894,11 +59869,11 @@
       <c r="N1629" s="48" t="s">
         <v>621</v>
       </c>
-      <c r="S1629" s="1" t="s">
+      <c r="S1629" s="8" t="s">
         <v>100</v>
       </c>
-      <c r="T1629" s="1" t="s">
-        <v>1499</v>
+      <c r="T1629" s="8" t="s">
+        <v>1496</v>
       </c>
       <c r="V1629" s="48"/>
     </row>
@@ -60666,9 +60641,6 @@
       <c r="O1659" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="U1659" s="1" t="s">
-        <v>1494</v>
-      </c>
       <c r="V1659" s="48"/>
     </row>
     <row r="1660" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -60773,9 +60745,6 @@
       <c r="O1663" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="U1663" s="1" t="s">
-        <v>1494</v>
-      </c>
       <c r="V1663" s="48" t="s">
         <v>1285</v>
       </c>
@@ -61684,14 +61653,14 @@
         <f t="shared" si="80"/>
         <v>99</v>
       </c>
-      <c r="N1699" s="48" t="s">
+      <c r="N1699" s="52" t="s">
         <v>277</v>
       </c>
       <c r="P1699" s="8" t="s">
         <v>74</v>
       </c>
       <c r="V1699" s="48" t="s">
-        <v>1434</v>
+        <v>1433</v>
       </c>
     </row>
     <row r="1700" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -62697,7 +62666,7 @@
       </c>
     </row>
     <row r="1740" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1740" s="2" t="s">
+      <c r="A1740" s="61" t="s">
         <v>87</v>
       </c>
       <c r="F1740" s="53" t="s">
@@ -62730,7 +62699,7 @@
       <c r="V1740" s="48"/>
     </row>
     <row r="1741" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1741" s="2" t="s">
+      <c r="A1741" s="61" t="s">
         <v>87</v>
       </c>
       <c r="F1741" s="53" t="s">
@@ -63148,9 +63117,6 @@
       <c r="O1756" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="U1756" s="1" t="s">
-        <v>1494</v>
-      </c>
       <c r="V1756" s="48"/>
     </row>
     <row r="1757" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -64080,6 +64046,12 @@
       <c r="N1793" s="48" t="s">
         <v>285</v>
       </c>
+      <c r="Q1793" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="R1793" s="1" t="s">
+        <v>121</v>
+      </c>
       <c r="V1793" s="48"/>
     </row>
     <row r="1794" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -64392,9 +64364,6 @@
       <c r="N1805" s="48" t="s">
         <v>716</v>
       </c>
-      <c r="U1805" s="1" t="s">
-        <v>1494</v>
-      </c>
       <c r="V1805" s="48"/>
     </row>
     <row r="1806" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -64494,9 +64463,6 @@
       <c r="N1809" s="48" t="s">
         <v>718</v>
       </c>
-      <c r="U1809" s="1" t="s">
-        <v>1493</v>
-      </c>
       <c r="V1809" s="48"/>
     </row>
     <row r="1810" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -65647,7 +65613,7 @@
         <v>156</v>
       </c>
       <c r="N1855" s="48" t="s">
-        <v>1512</v>
+        <v>1505</v>
       </c>
       <c r="O1855" s="8" t="s">
         <v>73</v>
@@ -66036,9 +66002,6 @@
       <c r="N1870" s="48" t="s">
         <v>285</v>
       </c>
-      <c r="T1870" s="1" t="s">
-        <v>1500</v>
-      </c>
       <c r="V1870" s="48"/>
     </row>
     <row r="1871" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -66072,6 +66035,9 @@
       <c r="S1871" s="1" t="s">
         <v>100</v>
       </c>
+      <c r="T1871" s="1" t="s">
+        <v>1508</v>
+      </c>
       <c r="V1871" s="48" t="s">
         <v>1305</v>
       </c>
@@ -66104,9 +66070,6 @@
       <c r="O1872" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="U1872" s="1" t="s">
-        <v>1494</v>
-      </c>
       <c r="V1872" s="48"/>
     </row>
     <row r="1873" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -66185,7 +66148,7 @@
         <v>176</v>
       </c>
       <c r="N1875" s="48" t="s">
-        <v>1512</v>
+        <v>1505</v>
       </c>
       <c r="O1875" s="8" t="s">
         <v>73</v>
@@ -67023,14 +66986,14 @@
         <f t="shared" si="89"/>
         <v>208</v>
       </c>
-      <c r="N1907" s="48" t="s">
+      <c r="N1907" s="52" t="s">
         <v>201</v>
       </c>
       <c r="P1907" s="8" t="s">
         <v>74</v>
       </c>
       <c r="V1907" s="48" t="s">
-        <v>1435</v>
+        <v>1434</v>
       </c>
     </row>
     <row r="1908" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -67125,9 +67088,6 @@
       <c r="N1911" s="48" t="s">
         <v>750</v>
       </c>
-      <c r="U1911" s="1" t="s">
-        <v>1494</v>
-      </c>
       <c r="V1911" s="48"/>
     </row>
     <row r="1912" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -67599,9 +67559,6 @@
       <c r="N1930" s="48" t="s">
         <v>765</v>
       </c>
-      <c r="U1930" s="1" t="s">
-        <v>1494</v>
-      </c>
       <c r="V1930" s="48"/>
     </row>
     <row r="1931" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -67926,14 +67883,14 @@
         <f t="shared" si="92"/>
         <v>36</v>
       </c>
-      <c r="N1943" s="48" t="s">
+      <c r="N1943" s="59" t="s">
         <v>1385</v>
       </c>
       <c r="P1943" s="8" t="s">
         <v>74</v>
       </c>
       <c r="V1943" s="48" t="s">
-        <v>1436</v>
+        <v>1435</v>
       </c>
     </row>
     <row r="1944" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -68899,14 +68856,14 @@
         <f t="shared" si="92"/>
         <v>40</v>
       </c>
-      <c r="N1983" s="48" t="s">
+      <c r="N1983" s="59" t="s">
         <v>776</v>
       </c>
       <c r="P1983" s="8" t="s">
         <v>74</v>
       </c>
       <c r="V1983" s="48" t="s">
-        <v>1437</v>
+        <v>1436</v>
       </c>
     </row>
     <row r="1984" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -69635,7 +69592,7 @@
         <v>74</v>
       </c>
       <c r="V2012" s="48" t="s">
-        <v>1437</v>
+        <v>1436</v>
       </c>
     </row>
     <row r="2013" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -69739,7 +69696,7 @@
       <c r="V2016" s="48"/>
     </row>
     <row r="2017" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A2017" s="2" t="s">
+      <c r="A2017" s="8" t="s">
         <v>87</v>
       </c>
       <c r="H2017" s="51" t="s">
@@ -69772,7 +69729,7 @@
       <c r="V2017" s="48"/>
     </row>
     <row r="2018" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A2018" s="2" t="s">
+      <c r="A2018" s="8" t="s">
         <v>87</v>
       </c>
       <c r="H2018" s="51" t="s">
@@ -69799,9 +69756,6 @@
       <c r="N2018" s="48" t="s">
         <v>811</v>
       </c>
-      <c r="U2018" s="1" t="s">
-        <v>1494</v>
-      </c>
       <c r="V2018" s="48"/>
     </row>
     <row r="2019" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -69833,7 +69787,7 @@
         <v>74</v>
       </c>
       <c r="V2019" s="48" t="s">
-        <v>1438</v>
+        <v>1437</v>
       </c>
     </row>
     <row r="2020" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -69934,7 +69888,7 @@
         <v>74</v>
       </c>
       <c r="V2023" s="48" t="s">
-        <v>1439</v>
+        <v>1438</v>
       </c>
     </row>
     <row r="2024" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -70183,7 +70137,7 @@
         <v>74</v>
       </c>
       <c r="V2032" s="48" t="s">
-        <v>1440</v>
+        <v>1439</v>
       </c>
     </row>
     <row r="2033" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -70268,9 +70222,6 @@
       <c r="O2035" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="U2035" s="1" t="s">
-        <v>1493</v>
-      </c>
       <c r="V2035" s="48" t="s">
         <v>1324</v>
       </c>
@@ -70457,7 +70408,7 @@
         <v>74</v>
       </c>
       <c r="V2042" s="48" t="s">
-        <v>1441</v>
+        <v>1440</v>
       </c>
     </row>
     <row r="2043" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -70482,14 +70433,11 @@
         <f t="shared" si="95"/>
         <v>31</v>
       </c>
-      <c r="N2043" s="48" t="s">
+      <c r="N2043" s="52" t="s">
         <v>543</v>
       </c>
       <c r="O2043" s="8" t="s">
         <v>76</v>
-      </c>
-      <c r="U2043" s="1" t="s">
-        <v>1494</v>
       </c>
       <c r="V2043" s="48"/>
     </row>
@@ -70515,7 +70463,7 @@
         <f t="shared" si="95"/>
         <v>32</v>
       </c>
-      <c r="N2044" s="48" t="s">
+      <c r="N2044" s="52" t="s">
         <v>827</v>
       </c>
       <c r="V2044" s="48"/>
@@ -70762,7 +70710,7 @@
         <v>74</v>
       </c>
       <c r="V2053" s="48" t="s">
-        <v>1442</v>
+        <v>1441</v>
       </c>
     </row>
     <row r="2054" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -71031,7 +70979,7 @@
         <v>74</v>
       </c>
       <c r="V2064" s="48" t="s">
-        <v>1443</v>
+        <v>1442</v>
       </c>
     </row>
     <row r="2065" spans="7:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -71779,7 +71727,7 @@
         <v>74</v>
       </c>
       <c r="V2093" s="48" t="s">
-        <v>1437</v>
+        <v>1436</v>
       </c>
     </row>
     <row r="2094" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -72012,7 +71960,7 @@
         <v>74</v>
       </c>
       <c r="V2102" s="48" t="s">
-        <v>1444</v>
+        <v>1443</v>
       </c>
     </row>
     <row r="2103" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -72195,7 +72143,7 @@
         <v>74</v>
       </c>
       <c r="V2109" s="48" t="s">
-        <v>1445</v>
+        <v>1444</v>
       </c>
     </row>
     <row r="2110" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -72355,9 +72303,6 @@
       <c r="N2115" s="48" t="s">
         <v>875</v>
       </c>
-      <c r="U2115" s="1" t="s">
-        <v>1494</v>
-      </c>
       <c r="V2115" s="48"/>
     </row>
     <row r="2116" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -72434,7 +72379,7 @@
         <v>74</v>
       </c>
       <c r="V2118" s="48" t="s">
-        <v>1446</v>
+        <v>1445</v>
       </c>
     </row>
     <row r="2119" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -72484,7 +72429,7 @@
         <v>878</v>
       </c>
       <c r="U2120" s="1" t="s">
-        <v>1501</v>
+        <v>1502</v>
       </c>
       <c r="V2120" s="48"/>
     </row>
@@ -72682,7 +72627,7 @@
         <v>74</v>
       </c>
       <c r="V2128" s="48" t="s">
-        <v>1447</v>
+        <v>1446</v>
       </c>
     </row>
     <row r="2129" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -72903,7 +72848,7 @@
         <v>74</v>
       </c>
       <c r="V2137" s="48" t="s">
-        <v>1446</v>
+        <v>1445</v>
       </c>
     </row>
     <row r="2138" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -72955,9 +72900,6 @@
       <c r="O2139" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="U2139" s="1" t="s">
-        <v>1494</v>
-      </c>
       <c r="V2139" s="48" t="s">
         <v>1338</v>
       </c>
@@ -73117,7 +73059,7 @@
         <v>74</v>
       </c>
       <c r="V2145" s="48" t="s">
-        <v>1448</v>
+        <v>1447</v>
       </c>
     </row>
     <row r="2146" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -73327,7 +73269,7 @@
         <v>74</v>
       </c>
       <c r="V2153" s="48" t="s">
-        <v>1449</v>
+        <v>1448</v>
       </c>
     </row>
     <row r="2154" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -73507,8 +73449,11 @@
       <c r="N2160" s="48" t="s">
         <v>906</v>
       </c>
-      <c r="U2160" s="1" t="s">
-        <v>1502</v>
+      <c r="S2160" s="8" t="s">
+        <v>1494</v>
+      </c>
+      <c r="T2160" s="8" t="s">
+        <v>1509</v>
       </c>
       <c r="V2160" s="48"/>
     </row>
@@ -73642,7 +73587,7 @@
         <v>74</v>
       </c>
       <c r="V2165" s="48" t="s">
-        <v>1450</v>
+        <v>1449</v>
       </c>
     </row>
     <row r="2166" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -73988,10 +73933,10 @@
         <v>913</v>
       </c>
       <c r="S2179" s="1" t="s">
-        <v>1505</v>
+        <v>1499</v>
       </c>
       <c r="T2179" s="1" t="s">
-        <v>1506</v>
+        <v>1500</v>
       </c>
       <c r="V2179" s="48"/>
     </row>
@@ -74024,10 +73969,10 @@
         <v>76</v>
       </c>
       <c r="S2180" s="1" t="s">
-        <v>1503</v>
+        <v>1497</v>
       </c>
       <c r="T2180" s="1" t="s">
-        <v>1504</v>
+        <v>1498</v>
       </c>
       <c r="V2180" s="48"/>
     </row>
@@ -74060,7 +74005,7 @@
         <v>74</v>
       </c>
       <c r="V2181" s="48" t="s">
-        <v>1451</v>
+        <v>1450</v>
       </c>
     </row>
     <row r="2182" spans="5:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -74284,7 +74229,7 @@
         <v>74</v>
       </c>
       <c r="V2190" s="48" t="s">
-        <v>1452</v>
+        <v>1451</v>
       </c>
     </row>
     <row r="2191" spans="5:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -74481,7 +74426,7 @@
         <v>74</v>
       </c>
       <c r="V2198" s="48" t="s">
-        <v>1453</v>
+        <v>1452</v>
       </c>
     </row>
     <row r="2199" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -74659,7 +74604,7 @@
         <v>74</v>
       </c>
       <c r="V2205" s="48" t="s">
-        <v>1454</v>
+        <v>1453</v>
       </c>
     </row>
     <row r="2206" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -74808,7 +74753,7 @@
         <v>74</v>
       </c>
       <c r="V2211" s="48" t="s">
-        <v>1455</v>
+        <v>1454</v>
       </c>
     </row>
     <row r="2212" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -75028,14 +74973,14 @@
       <c r="P2220" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="S2220" s="1" t="s">
-        <v>1497</v>
-      </c>
-      <c r="T2220" s="1" t="s">
-        <v>1507</v>
+      <c r="S2220" s="8" t="s">
+        <v>1494</v>
+      </c>
+      <c r="T2220" s="8" t="s">
+        <v>1501</v>
       </c>
       <c r="V2220" s="48" t="s">
-        <v>1456</v>
+        <v>1455</v>
       </c>
     </row>
     <row r="2221" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -75237,7 +75182,7 @@
         <v>74</v>
       </c>
       <c r="V2228" s="48" t="s">
-        <v>1457</v>
+        <v>1456</v>
       </c>
     </row>
     <row r="2229" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -75384,14 +75329,14 @@
       <c r="P2234" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="S2234" s="1" t="s">
-        <v>1497</v>
-      </c>
-      <c r="T2234" s="1" t="s">
-        <v>1507</v>
+      <c r="S2234" s="8" t="s">
+        <v>1494</v>
+      </c>
+      <c r="T2234" s="8" t="s">
+        <v>1501</v>
       </c>
       <c r="V2234" s="48" t="s">
-        <v>1458</v>
+        <v>1457</v>
       </c>
     </row>
     <row r="2235" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -75545,7 +75490,7 @@
         <v>74</v>
       </c>
       <c r="V2240" s="48" t="s">
-        <v>1459</v>
+        <v>1458</v>
       </c>
     </row>
     <row r="2241" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -75766,7 +75711,7 @@
         <v>74</v>
       </c>
       <c r="V2249" s="48" t="s">
-        <v>1460</v>
+        <v>1459</v>
       </c>
     </row>
     <row r="2250" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -75993,7 +75938,7 @@
         <v>74</v>
       </c>
       <c r="V2258" s="48" t="s">
-        <v>1461</v>
+        <v>1460</v>
       </c>
     </row>
     <row r="2259" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -76214,7 +76159,7 @@
         <v>74</v>
       </c>
       <c r="V2267" s="48" t="s">
-        <v>1460</v>
+        <v>1459</v>
       </c>
     </row>
     <row r="2268" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -76465,7 +76410,7 @@
         <v>74</v>
       </c>
       <c r="V2277" s="48" t="s">
-        <v>1461</v>
+        <v>1460</v>
       </c>
     </row>
     <row r="2278" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -76491,9 +76436,6 @@
       <c r="N2278" s="52" t="s">
         <v>942</v>
       </c>
-      <c r="U2278" s="1" t="s">
-        <v>1508</v>
-      </c>
       <c r="V2278" s="48"/>
     </row>
     <row r="2279" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -76521,7 +76463,7 @@
       <c r="N2279" s="52" t="s">
         <v>943</v>
       </c>
-      <c r="U2279" s="1" t="s">
+      <c r="U2279" s="58" t="s">
         <v>111</v>
       </c>
       <c r="V2279" s="48"/>
@@ -76690,7 +76632,7 @@
         <v>74</v>
       </c>
       <c r="V2285" s="48" t="s">
-        <v>1462</v>
+        <v>1461</v>
       </c>
     </row>
     <row r="2286" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -76742,11 +76684,8 @@
       <c r="P2287" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="U2287" s="1" t="s">
-        <v>1509</v>
-      </c>
       <c r="V2287" s="48" t="s">
-        <v>1463</v>
+        <v>1462</v>
       </c>
     </row>
     <row r="2288" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -76937,7 +76876,7 @@
         <v>74</v>
       </c>
       <c r="V2294" s="48" t="s">
-        <v>1464</v>
+        <v>1463</v>
       </c>
     </row>
     <row r="2295" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -77348,7 +77287,7 @@
         <v>74</v>
       </c>
       <c r="V2309" s="48" t="s">
-        <v>1465</v>
+        <v>1464</v>
       </c>
     </row>
     <row r="2310" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -77711,7 +77650,7 @@
         <v>74</v>
       </c>
       <c r="V2322" s="48" t="s">
-        <v>1466</v>
+        <v>1465</v>
       </c>
     </row>
     <row r="2323" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -77867,7 +77806,7 @@
         <v>74</v>
       </c>
       <c r="V2328" s="48" t="s">
-        <v>1467</v>
+        <v>1466</v>
       </c>
     </row>
     <row r="2329" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -77943,11 +77882,8 @@
       <c r="P2331" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="U2331" s="1" t="s">
-        <v>1493</v>
-      </c>
       <c r="V2331" s="48" t="s">
-        <v>1468</v>
+        <v>1467</v>
       </c>
     </row>
     <row r="2332" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -78099,7 +78035,7 @@
         <v>74</v>
       </c>
       <c r="V2337" s="48" t="s">
-        <v>1469</v>
+        <v>1468</v>
       </c>
     </row>
     <row r="2338" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -78124,9 +78060,6 @@
       <c r="N2338" s="48" t="s">
         <v>942</v>
       </c>
-      <c r="U2338" s="1" t="s">
-        <v>1508</v>
-      </c>
       <c r="V2338" s="48"/>
     </row>
     <row r="2339" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -78151,7 +78084,7 @@
       <c r="N2339" s="48" t="s">
         <v>943</v>
       </c>
-      <c r="U2339" s="1" t="s">
+      <c r="U2339" s="58" t="s">
         <v>111</v>
       </c>
       <c r="V2339" s="48"/>
@@ -78302,7 +78235,7 @@
         <v>74</v>
       </c>
       <c r="V2345" s="48" t="s">
-        <v>1462</v>
+        <v>1461</v>
       </c>
     </row>
     <row r="2346" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -78355,7 +78288,7 @@
         <v>74</v>
       </c>
       <c r="V2347" s="48" t="s">
-        <v>1463</v>
+        <v>1462</v>
       </c>
     </row>
     <row r="2348" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -78536,7 +78469,7 @@
         <v>74</v>
       </c>
       <c r="V2354" s="48" t="s">
-        <v>1470</v>
+        <v>1469</v>
       </c>
     </row>
     <row r="2355" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -78733,7 +78666,7 @@
         <v>74</v>
       </c>
       <c r="V2362" s="48" t="s">
-        <v>1470</v>
+        <v>1469</v>
       </c>
     </row>
     <row r="2363" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -78758,9 +78691,7 @@
       <c r="N2363" s="48" t="s">
         <v>942</v>
       </c>
-      <c r="U2363" s="59" t="s">
-        <v>1508</v>
-      </c>
+      <c r="U2363" s="58"/>
       <c r="V2363" s="48"/>
     </row>
     <row r="2364" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -78785,7 +78716,7 @@
       <c r="N2364" s="48" t="s">
         <v>943</v>
       </c>
-      <c r="U2364" s="59" t="s">
+      <c r="U2364" s="58" t="s">
         <v>111</v>
       </c>
       <c r="V2364" s="48"/>
@@ -78936,7 +78867,7 @@
         <v>74</v>
       </c>
       <c r="V2370" s="48" t="s">
-        <v>1462</v>
+        <v>1461</v>
       </c>
     </row>
     <row r="2371" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -78988,11 +78919,8 @@
       <c r="P2372" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="U2372" s="1" t="s">
-        <v>1493</v>
-      </c>
       <c r="V2372" s="48" t="s">
-        <v>1463</v>
+        <v>1462</v>
       </c>
     </row>
     <row r="2373" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -79188,7 +79116,7 @@
         <v>74</v>
       </c>
       <c r="V2380" s="48" t="s">
-        <v>1471</v>
+        <v>1470</v>
       </c>
     </row>
     <row r="2381" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -79264,9 +79192,6 @@
       <c r="O2383" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="U2383" s="1" t="s">
-        <v>1493</v>
-      </c>
       <c r="V2383" s="48" t="s">
         <v>1353</v>
       </c>
@@ -79345,7 +79270,7 @@
         <v>74</v>
       </c>
       <c r="V2386" s="48" t="s">
-        <v>1472</v>
+        <v>1471</v>
       </c>
     </row>
     <row r="2387" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -79367,12 +79292,10 @@
         <f t="shared" si="113"/>
         <v>110</v>
       </c>
-      <c r="N2387" s="48" t="s">
+      <c r="N2387" s="52" t="s">
         <v>942</v>
       </c>
-      <c r="U2387" s="59" t="s">
-        <v>1508</v>
-      </c>
+      <c r="U2387" s="62"/>
       <c r="V2387" s="48"/>
     </row>
     <row r="2388" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -79394,10 +79317,10 @@
         <f t="shared" si="113"/>
         <v>111</v>
       </c>
-      <c r="N2388" s="48" t="s">
+      <c r="N2388" s="52" t="s">
         <v>943</v>
       </c>
-      <c r="U2388" s="59" t="s">
+      <c r="U2388" s="58" t="s">
         <v>111</v>
       </c>
       <c r="V2388" s="48"/>
@@ -79421,7 +79344,7 @@
         <f t="shared" si="113"/>
         <v>112</v>
       </c>
-      <c r="N2389" s="48" t="s">
+      <c r="N2389" s="52" t="s">
         <v>944</v>
       </c>
       <c r="V2389" s="48"/>
@@ -79548,7 +79471,7 @@
         <v>74</v>
       </c>
       <c r="V2394" s="48" t="s">
-        <v>1462</v>
+        <v>1461</v>
       </c>
     </row>
     <row r="2395" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -79600,11 +79523,8 @@
       <c r="P2396" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="U2396" s="1" t="s">
-        <v>1493</v>
-      </c>
       <c r="V2396" s="48" t="s">
-        <v>1463</v>
+        <v>1462</v>
       </c>
     </row>
     <row r="2397" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -79758,7 +79678,7 @@
         <v>74</v>
       </c>
       <c r="V2402" s="48" t="s">
-        <v>1473</v>
+        <v>1472</v>
       </c>
     </row>
     <row r="2403" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -79915,7 +79835,7 @@
         <v>74</v>
       </c>
       <c r="V2408" s="48" t="s">
-        <v>1474</v>
+        <v>1473</v>
       </c>
     </row>
     <row r="2409" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -79937,12 +79857,10 @@
         <f t="shared" si="113"/>
         <v>132</v>
       </c>
-      <c r="N2409" s="48" t="s">
+      <c r="N2409" s="52" t="s">
         <v>942</v>
       </c>
-      <c r="U2409" s="59" t="s">
-        <v>1508</v>
-      </c>
+      <c r="U2409" s="58"/>
       <c r="V2409" s="48"/>
     </row>
     <row r="2410" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -79964,10 +79882,10 @@
         <f t="shared" si="113"/>
         <v>133</v>
       </c>
-      <c r="N2410" s="48" t="s">
+      <c r="N2410" s="52" t="s">
         <v>943</v>
       </c>
-      <c r="U2410" s="59" t="s">
+      <c r="U2410" s="58" t="s">
         <v>111</v>
       </c>
       <c r="V2410" s="48"/>
@@ -79991,7 +79909,7 @@
         <f t="shared" si="113"/>
         <v>134</v>
       </c>
-      <c r="N2411" s="48" t="s">
+      <c r="N2411" s="52" t="s">
         <v>944</v>
       </c>
       <c r="V2411" s="48"/>
@@ -80118,7 +80036,7 @@
         <v>74</v>
       </c>
       <c r="V2416" s="48" t="s">
-        <v>1462</v>
+        <v>1461</v>
       </c>
     </row>
     <row r="2417" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -80171,7 +80089,7 @@
         <v>74</v>
       </c>
       <c r="V2418" s="48" t="s">
-        <v>1463</v>
+        <v>1462</v>
       </c>
     </row>
     <row r="2419" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -80416,7 +80334,7 @@
         <v>74</v>
       </c>
       <c r="V2427" s="48" t="s">
-        <v>1475</v>
+        <v>1474</v>
       </c>
     </row>
     <row r="2428" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -80615,7 +80533,7 @@
         <v>74</v>
       </c>
       <c r="V2435" s="48" t="s">
-        <v>1476</v>
+        <v>1475</v>
       </c>
     </row>
     <row r="2436" spans="2:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -80769,7 +80687,7 @@
         <v>74</v>
       </c>
       <c r="V2440" s="48" t="s">
-        <v>1477</v>
+        <v>1476</v>
       </c>
     </row>
     <row r="2441" spans="2:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -80917,6 +80835,12 @@
       <c r="N2446" s="48" t="s">
         <v>904</v>
       </c>
+      <c r="S2446" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="T2446" s="8" t="s">
+        <v>1498</v>
+      </c>
       <c r="V2446" s="48"/>
     </row>
     <row r="2447" spans="2:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -80941,6 +80865,8 @@
       <c r="N2447" s="48" t="s">
         <v>1009</v>
       </c>
+      <c r="S2447" s="8"/>
+      <c r="T2447" s="8"/>
       <c r="V2447" s="48"/>
     </row>
     <row r="2448" spans="2:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -80968,8 +80894,10 @@
       <c r="P2448" s="8" t="s">
         <v>74</v>
       </c>
+      <c r="S2448" s="8"/>
+      <c r="T2448" s="8"/>
       <c r="V2448" s="48" t="s">
-        <v>1478</v>
+        <v>1477</v>
       </c>
     </row>
     <row r="2449" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -80997,6 +80925,8 @@
       <c r="N2449" s="48" t="s">
         <v>1010</v>
       </c>
+      <c r="S2449" s="8"/>
+      <c r="T2449" s="8"/>
       <c r="V2449" s="48"/>
     </row>
     <row r="2450" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -81027,6 +80957,8 @@
       <c r="N2450" s="48" t="s">
         <v>249</v>
       </c>
+      <c r="S2450" s="8"/>
+      <c r="T2450" s="8"/>
       <c r="V2450" s="48"/>
     </row>
     <row r="2451" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -81060,10 +80992,10 @@
       <c r="N2451" s="48" t="s">
         <v>1011</v>
       </c>
-      <c r="S2451" s="1" t="s">
+      <c r="S2451" s="8" t="s">
         <v>126</v>
       </c>
-      <c r="T2451" s="1" t="s">
+      <c r="T2451" s="8" t="s">
         <v>127</v>
       </c>
       <c r="V2451" s="48"/>
@@ -81207,7 +81139,7 @@
         <v>74</v>
       </c>
       <c r="V2456" s="48" t="s">
-        <v>1479</v>
+        <v>1478</v>
       </c>
     </row>
     <row r="2457" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -81284,7 +81216,7 @@
         <v>74</v>
       </c>
       <c r="V2459" s="48" t="s">
-        <v>1480</v>
+        <v>1479</v>
       </c>
     </row>
     <row r="2460" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -81486,7 +81418,7 @@
         <v>74</v>
       </c>
       <c r="V2467" s="48" t="s">
-        <v>1481</v>
+        <v>1480</v>
       </c>
     </row>
     <row r="2468" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -81563,7 +81495,7 @@
         <v>74</v>
       </c>
       <c r="V2470" s="48" t="s">
-        <v>1482</v>
+        <v>1481</v>
       </c>
     </row>
     <row r="2471" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -81736,7 +81668,7 @@
         <v>74</v>
       </c>
       <c r="V2477" s="48" t="s">
-        <v>1483</v>
+        <v>1482</v>
       </c>
     </row>
     <row r="2478" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -81830,14 +81762,14 @@
         <f t="shared" si="116"/>
         <v>204</v>
       </c>
-      <c r="N2481" s="48" t="s">
+      <c r="N2481" s="59" t="s">
         <v>904</v>
       </c>
       <c r="P2481" s="8" t="s">
         <v>74</v>
       </c>
       <c r="V2481" s="48" t="s">
-        <v>1481</v>
+        <v>1480</v>
       </c>
     </row>
     <row r="2482" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -81908,6 +81840,12 @@
       <c r="N2484" s="48" t="s">
         <v>1028</v>
       </c>
+      <c r="S2484" s="8" t="s">
+        <v>1494</v>
+      </c>
+      <c r="T2484" s="8" t="s">
+        <v>1510</v>
+      </c>
       <c r="V2484" s="48"/>
     </row>
     <row r="2485" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -82340,7 +82278,7 @@
       <c r="N2502" s="48" t="s">
         <v>1035</v>
       </c>
-      <c r="U2502" s="1" t="s">
+      <c r="U2502" s="8" t="s">
         <v>119</v>
       </c>
       <c r="V2502" s="48"/>
@@ -82367,7 +82305,7 @@
       <c r="N2503" s="48" t="s">
         <v>1036</v>
       </c>
-      <c r="U2503" s="1" t="s">
+      <c r="U2503" s="8" t="s">
         <v>119</v>
       </c>
       <c r="V2503" s="48"/>
@@ -82446,7 +82384,7 @@
         <v>74</v>
       </c>
       <c r="V2506" s="48" t="s">
-        <v>1484</v>
+        <v>1483</v>
       </c>
     </row>
     <row r="2507" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -82567,11 +82505,11 @@
       <c r="N2511" s="48" t="s">
         <v>1039</v>
       </c>
-      <c r="S2511" s="1" t="s">
-        <v>1497</v>
-      </c>
-      <c r="T2511" s="1" t="s">
-        <v>1510</v>
+      <c r="S2511" s="8" t="s">
+        <v>1494</v>
+      </c>
+      <c r="T2511" s="8" t="s">
+        <v>1503</v>
       </c>
       <c r="V2511" s="48"/>
     </row>
@@ -82676,7 +82614,7 @@
         <v>74</v>
       </c>
       <c r="V2515" s="48" t="s">
-        <v>1481</v>
+        <v>1480</v>
       </c>
     </row>
     <row r="2516" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -82771,13 +82709,13 @@
         <v>38</v>
       </c>
       <c r="N2519" s="48" t="s">
-        <v>1423</v>
+        <v>1511</v>
       </c>
       <c r="P2519" s="8" t="s">
         <v>74</v>
       </c>
       <c r="V2519" s="48" t="s">
-        <v>1485</v>
+        <v>1484</v>
       </c>
     </row>
     <row r="2520" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -83009,9 +82947,6 @@
       <c r="N2528" s="48" t="s">
         <v>1049</v>
       </c>
-      <c r="U2528" s="1" t="s">
-        <v>1494</v>
-      </c>
       <c r="V2528" s="48"/>
     </row>
     <row r="2529" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -83037,7 +82972,7 @@
         <v>48</v>
       </c>
       <c r="N2529" s="48" t="s">
-        <v>1424</v>
+        <v>1423</v>
       </c>
       <c r="O2529" s="8" t="s">
         <v>73</v>
@@ -83046,7 +82981,7 @@
         <v>74</v>
       </c>
       <c r="V2529" s="48" t="s">
-        <v>1486</v>
+        <v>1485</v>
       </c>
     </row>
     <row r="2530" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -83192,13 +83127,13 @@
         <v>54</v>
       </c>
       <c r="N2535" s="48" t="s">
-        <v>1425</v>
+        <v>1424</v>
       </c>
       <c r="P2535" s="8" t="s">
         <v>74</v>
       </c>
       <c r="V2535" s="48" t="s">
-        <v>1487</v>
+        <v>1486</v>
       </c>
     </row>
     <row r="2536" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -83269,13 +83204,13 @@
         <v>57</v>
       </c>
       <c r="N2538" s="48" t="s">
-        <v>1426</v>
+        <v>1425</v>
       </c>
       <c r="P2538" s="8" t="s">
         <v>74</v>
       </c>
       <c r="V2538" s="48" t="s">
-        <v>1488</v>
+        <v>1487</v>
       </c>
     </row>
     <row r="2539" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -83428,13 +83363,13 @@
         <v>63</v>
       </c>
       <c r="N2544" s="48" t="s">
-        <v>1427</v>
+        <v>1426</v>
       </c>
       <c r="P2544" s="8" t="s">
         <v>74</v>
       </c>
       <c r="V2544" s="48" t="s">
-        <v>1489</v>
+        <v>1488</v>
       </c>
     </row>
     <row r="2545" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -83510,7 +83445,7 @@
         <v>66</v>
       </c>
       <c r="N2547" s="48" t="s">
-        <v>1428</v>
+        <v>1427</v>
       </c>
       <c r="O2547" s="8" t="s">
         <v>73</v>
@@ -83519,7 +83454,7 @@
         <v>74</v>
       </c>
       <c r="V2547" s="48" t="s">
-        <v>1490</v>
+        <v>1489</v>
       </c>
     </row>
     <row r="2548" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -83592,9 +83527,6 @@
       <c r="N2550" s="48" t="s">
         <v>1065</v>
       </c>
-      <c r="U2550" s="1" t="s">
-        <v>1509</v>
-      </c>
       <c r="V2550" s="48"/>
     </row>
     <row r="2551" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -83665,16 +83597,16 @@
         <v>72</v>
       </c>
       <c r="N2553" s="48" t="s">
-        <v>1429</v>
+        <v>1428</v>
       </c>
       <c r="P2553" s="8" t="s">
         <v>74</v>
       </c>
       <c r="U2553" s="1" t="s">
-        <v>1493</v>
+        <v>119</v>
       </c>
       <c r="V2553" s="48" t="s">
-        <v>1491</v>
+        <v>1490</v>
       </c>
     </row>
     <row r="2554" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -83753,13 +83685,13 @@
         <v>75</v>
       </c>
       <c r="N2556" s="48" t="s">
-        <v>1430</v>
+        <v>1429</v>
       </c>
       <c r="P2556" s="8" t="s">
         <v>74</v>
       </c>
       <c r="V2556" s="48" t="s">
-        <v>1492</v>
+        <v>1491</v>
       </c>
     </row>
     <row r="2557" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -84479,7 +84411,7 @@
         <v>74</v>
       </c>
       <c r="V2584" s="48" t="s">
-        <v>1437</v>
+        <v>1436</v>
       </c>
     </row>
     <row r="2585" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -85437,14 +85369,14 @@
         <f t="shared" si="122"/>
         <v>38</v>
       </c>
-      <c r="N2622" s="60" t="s">
+      <c r="N2622" s="59" t="s">
         <v>776</v>
       </c>
       <c r="P2622" s="8" t="s">
         <v>74</v>
       </c>
       <c r="V2622" s="48" t="s">
-        <v>1437</v>
+        <v>1436</v>
       </c>
     </row>
     <row r="2623" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
nmv 27 02 2024
</commit_message>
<xml_diff>
--- a/TS Jatai Working/Padam Input Templates/TS 7.4 Padam Input Template.xlsx
+++ b/TS Jatai Working/Padam Input Templates/TS 7.4 Padam Input Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ALL IMP DATA\GitHub\texts\TS Jatai Working\Padam Input Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C3E1490-5173-48C9-A922-4A7ED6743995}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6B90EEE-4F24-4ACD-90C8-7C5F4EEFF5BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6994" uniqueCount="1512">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7003" uniqueCount="1512">
   <si>
     <t>Passage</t>
   </si>
@@ -4725,7 +4725,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -4753,6 +4753,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -4967,20 +4973,20 @@
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="24" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="3" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -5264,10 +5270,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V2728"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1028" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A1027" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="L1" sqref="L1"/>
-      <selection pane="bottomLeft" activeCell="K1042" sqref="K1042:U1042"/>
+      <selection pane="bottomLeft" activeCell="K1041" sqref="K1041:V1041"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.25"/>
@@ -7741,7 +7747,7 @@
         <f t="shared" si="2"/>
         <v>50</v>
       </c>
-      <c r="N51" s="62" t="s">
+      <c r="N51" s="48" t="s">
         <v>164</v>
       </c>
       <c r="O51" s="7"/>
@@ -11116,7 +11122,7 @@
         <f t="shared" si="8"/>
         <v>145</v>
       </c>
-      <c r="N146" s="62" t="s">
+      <c r="N146" s="48" t="s">
         <v>1381</v>
       </c>
       <c r="O146" s="8" t="s">
@@ -23678,7 +23684,7 @@
         <f t="shared" si="26"/>
         <v>100</v>
       </c>
-      <c r="N520" s="62" t="s">
+      <c r="N520" s="48" t="s">
         <v>172</v>
       </c>
       <c r="O520" s="7"/>
@@ -30615,7 +30621,7 @@
         <f t="shared" si="35"/>
         <v>8</v>
       </c>
-      <c r="N727" s="63" t="s">
+      <c r="N727" s="62" t="s">
         <v>407</v>
       </c>
       <c r="O727" s="7"/>
@@ -30649,10 +30655,12 @@
         <f t="shared" si="35"/>
         <v>9</v>
       </c>
-      <c r="N728" s="63" t="s">
+      <c r="N728" s="62" t="s">
         <v>408</v>
       </c>
-      <c r="O728" s="7"/>
+      <c r="O728" s="8" t="s">
+        <v>76</v>
+      </c>
       <c r="P728" s="8"/>
       <c r="Q728" s="8"/>
       <c r="R728" s="8"/>
@@ -33597,7 +33605,7 @@
         <f t="shared" si="38"/>
         <v>100</v>
       </c>
-      <c r="N819" s="62" t="s">
+      <c r="N819" s="48" t="s">
         <v>201</v>
       </c>
       <c r="O819" s="7"/>
@@ -37021,7 +37029,7 @@
         <f t="shared" si="44"/>
         <v>33</v>
       </c>
-      <c r="N924" s="64" t="s">
+      <c r="N924" s="63" t="s">
         <v>1511</v>
       </c>
       <c r="O924" s="8" t="s">
@@ -40855,31 +40863,31 @@
       <c r="J1041" s="9">
         <v>20</v>
       </c>
-      <c r="K1041" s="6">
+      <c r="K1041" s="64">
         <f t="shared" si="48"/>
         <v>1040</v>
       </c>
-      <c r="L1041" s="6">
+      <c r="L1041" s="64">
         <f t="shared" si="49"/>
         <v>50</v>
       </c>
-      <c r="M1041" s="6">
+      <c r="M1041" s="64">
         <f t="shared" si="50"/>
         <v>150</v>
       </c>
-      <c r="N1041" s="48" t="s">
+      <c r="N1041" s="65" t="s">
         <v>490</v>
       </c>
-      <c r="O1041" s="8" t="s">
+      <c r="O1041" s="66" t="s">
         <v>73</v>
       </c>
-      <c r="P1041" s="8"/>
-      <c r="Q1041" s="8"/>
-      <c r="R1041" s="8"/>
-      <c r="S1041" s="8"/>
-      <c r="T1041" s="8"/>
-      <c r="U1041" s="8"/>
-      <c r="V1041" s="48" t="s">
+      <c r="P1041" s="66"/>
+      <c r="Q1041" s="66"/>
+      <c r="R1041" s="66"/>
+      <c r="S1041" s="66"/>
+      <c r="T1041" s="66"/>
+      <c r="U1041" s="66"/>
+      <c r="V1041" s="65" t="s">
         <v>1219</v>
       </c>
     </row>
@@ -40890,27 +40898,27 @@
       <c r="J1042" s="9">
         <v>21</v>
       </c>
-      <c r="K1042" s="65">
+      <c r="K1042" s="6">
         <f t="shared" si="48"/>
         <v>1041</v>
       </c>
-      <c r="L1042" s="65">
+      <c r="L1042" s="6">
         <v>1</v>
       </c>
-      <c r="M1042" s="65">
+      <c r="M1042" s="6">
         <f t="shared" si="50"/>
         <v>151</v>
       </c>
-      <c r="N1042" s="66" t="s">
+      <c r="N1042" s="48" t="s">
         <v>149</v>
       </c>
-      <c r="O1042" s="12"/>
-      <c r="P1042" s="13"/>
-      <c r="Q1042" s="13"/>
-      <c r="R1042" s="13"/>
-      <c r="S1042" s="13"/>
-      <c r="T1042" s="13"/>
-      <c r="U1042" s="13"/>
+      <c r="O1042" s="7"/>
+      <c r="P1042" s="8"/>
+      <c r="Q1042" s="8"/>
+      <c r="R1042" s="8"/>
+      <c r="S1042" s="8"/>
+      <c r="T1042" s="8"/>
+      <c r="U1042" s="8"/>
       <c r="V1042" s="48"/>
     </row>
     <row r="1043" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -43070,7 +43078,7 @@
         <f t="shared" si="53"/>
         <v>217</v>
       </c>
-      <c r="N1108" s="59" t="s">
+      <c r="N1108" s="48" t="s">
         <v>1381</v>
       </c>
       <c r="O1108" s="8" t="s">
@@ -47444,7 +47452,7 @@
         <f t="shared" si="59"/>
         <v>136</v>
       </c>
-      <c r="N1244" s="59" t="s">
+      <c r="N1244" s="48" t="s">
         <v>1381</v>
       </c>
       <c r="O1244" s="8" t="s">
@@ -50713,7 +50721,7 @@
         <f t="shared" si="62"/>
         <v>100</v>
       </c>
-      <c r="N1344" s="59" t="s">
+      <c r="N1344" s="48" t="s">
         <v>337</v>
       </c>
       <c r="O1344" s="7"/>
@@ -56781,7 +56789,9 @@
       <c r="N1523" s="48" t="s">
         <v>542</v>
       </c>
-      <c r="O1523" s="7"/>
+      <c r="O1523" s="8" t="s">
+        <v>76</v>
+      </c>
       <c r="P1523" s="8"/>
       <c r="Q1523" s="8"/>
       <c r="R1523" s="8"/>
@@ -57151,7 +57161,9 @@
       <c r="N1534" s="52" t="s">
         <v>408</v>
       </c>
-      <c r="O1534" s="7"/>
+      <c r="O1534" s="8" t="s">
+        <v>76</v>
+      </c>
       <c r="P1534" s="8"/>
       <c r="Q1534" s="8"/>
       <c r="R1534" s="8"/>
@@ -57352,7 +57364,9 @@
       <c r="N1540" s="48" t="s">
         <v>408</v>
       </c>
-      <c r="O1540" s="7"/>
+      <c r="O1540" s="8" t="s">
+        <v>76</v>
+      </c>
       <c r="P1540" s="8"/>
       <c r="Q1540" s="8"/>
       <c r="R1540" s="8"/>
@@ -58907,6 +58921,9 @@
       <c r="N1591" s="48" t="s">
         <v>408</v>
       </c>
+      <c r="O1591" s="8" t="s">
+        <v>76</v>
+      </c>
       <c r="S1591" s="8" t="s">
         <v>83</v>
       </c>
@@ -60504,6 +60521,9 @@
       <c r="N1653" s="48" t="s">
         <v>542</v>
       </c>
+      <c r="O1653" s="8" t="s">
+        <v>76</v>
+      </c>
       <c r="V1653" s="48"/>
     </row>
     <row r="1654" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -62980,6 +63000,9 @@
       <c r="N1750" s="48" t="s">
         <v>542</v>
       </c>
+      <c r="O1750" s="8" t="s">
+        <v>76</v>
+      </c>
       <c r="V1750" s="48"/>
     </row>
     <row r="1751" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -67901,7 +67924,7 @@
         <f t="shared" si="92"/>
         <v>36</v>
       </c>
-      <c r="N1943" s="59" t="s">
+      <c r="N1943" s="48" t="s">
         <v>1384</v>
       </c>
       <c r="P1943" s="8" t="s">
@@ -68874,7 +68897,7 @@
         <f t="shared" si="92"/>
         <v>40</v>
       </c>
-      <c r="N1983" s="59" t="s">
+      <c r="N1983" s="48" t="s">
         <v>775</v>
       </c>
       <c r="P1983" s="8" t="s">
@@ -76839,6 +76862,9 @@
       <c r="N2292" s="48" t="s">
         <v>552</v>
       </c>
+      <c r="O2292" s="8" t="s">
+        <v>76</v>
+      </c>
       <c r="V2292" s="48"/>
     </row>
     <row r="2293" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -77249,6 +77275,9 @@
       </c>
       <c r="N2307" s="48" t="s">
         <v>552</v>
+      </c>
+      <c r="O2307" s="8" t="s">
+        <v>76</v>
       </c>
       <c r="V2307" s="48"/>
     </row>
@@ -81779,7 +81808,7 @@
         <f t="shared" si="116"/>
         <v>204</v>
       </c>
-      <c r="N2481" s="59" t="s">
+      <c r="N2481" s="48" t="s">
         <v>903</v>
       </c>
       <c r="P2481" s="8" t="s">

</xml_diff>